<commit_message>
Updated Excel files based on new neutron populations; deleted "set acelib" line in U233_MET_FAST_001 input file to test environment variables in Savio
</commit_message>
<xml_diff>
--- a/PU_MET_FAST_005/PU_MET_FAST_005.xlsx
+++ b/PU_MET_FAST_005/PU_MET_FAST_005.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\ML_neutronics\PU-MET-FAST-005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\ML_neutronics\PU_MET_FAST_005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03946796-2562-426C-A627-214B437502E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9300981D-1543-4D0A-89F8-68B994C53F08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12107" yWindow="2647" windowWidth="9600" windowHeight="4920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -684,16 +684,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>637752</xdr:colOff>
+      <xdr:colOff>636693</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>154093</xdr:rowOff>
+      <xdr:rowOff>149860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9F097EA-1B70-4CB8-B755-5CB485C6BF7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B26C8A85-F6D1-451F-BD1C-FAF02E4CA366}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -709,7 +709,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8636000" y="0"/>
+          <a:off x="8991600" y="0"/>
           <a:ext cx="1280160" cy="1280160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -728,16 +728,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>637752</xdr:colOff>
+      <xdr:colOff>636693</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>154093</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03EAAE1F-CCD1-4C9D-AB4B-ED64DC11F300}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34E587A3-0F60-4A3A-B2DA-C2A3895DEDCC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -753,7 +753,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8636000" y="1312333"/>
+          <a:off x="8991600" y="1312333"/>
           <a:ext cx="1280160" cy="1280160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1031,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1141,10 +1141,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="4">
-        <v>1.01231</v>
+        <v>1.01559</v>
       </c>
       <c r="C6" s="5">
-        <v>2.0600000000000002E-3</v>
+        <v>1.42E-3</v>
       </c>
       <c r="D6" s="38">
         <v>1.008</v>
@@ -1162,10 +1162,10 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7" s="37"/>
       <c r="B7" s="6">
-        <v>1.0102800000000001</v>
+        <v>1.0132399999999999</v>
       </c>
       <c r="C7" s="7">
-        <v>1.98E-3</v>
+        <v>1.4300000000000001E-3</v>
       </c>
       <c r="D7" s="38"/>
       <c r="E7" s="40"/>
@@ -1179,10 +1179,10 @@
     <row r="8" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="37"/>
       <c r="B8" s="6">
-        <v>2.0591400000000001E-3</v>
+        <v>2.1105400000000002E-3</v>
       </c>
       <c r="C8" s="7">
-        <v>4.9410000000000003E-2</v>
+        <v>3.5950000000000003E-2</v>
       </c>
       <c r="D8" s="38"/>
       <c r="E8" s="40"/>
@@ -1198,10 +1198,10 @@
         <v>13</v>
       </c>
       <c r="B9" s="6">
-        <v>1.0108699999999999</v>
+        <v>1.0143500000000001</v>
       </c>
       <c r="C9" s="7">
-        <v>1.2999999999999999E-3</v>
+        <v>1.0200000000000001E-3</v>
       </c>
       <c r="D9" s="38"/>
       <c r="E9" s="40"/>
@@ -1215,10 +1215,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="6">
-        <v>1.0110399999999999</v>
+        <v>1.0140899999999999</v>
       </c>
       <c r="C10" s="7">
-        <v>1.6000000000000001E-3</v>
+        <v>1.15E-3</v>
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="40"/>
@@ -1234,10 +1234,10 @@
         <v>15</v>
       </c>
       <c r="B11" s="6">
-        <v>1.0108699999999999</v>
+        <v>1.0143500000000001</v>
       </c>
       <c r="C11" s="7">
-        <v>1.2999999999999999E-3</v>
+        <v>1.0200000000000001E-3</v>
       </c>
       <c r="D11" s="39"/>
       <c r="E11" s="41"/>
@@ -1253,10 +1253,10 @@
         <v>16</v>
       </c>
       <c r="B12" s="10">
-        <v>2.7015699999999998</v>
+        <v>2.70316</v>
       </c>
       <c r="C12" s="11">
-        <v>4.0000000000000002E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="G12" s="23" t="s">
         <v>28</v>
@@ -1366,7 +1366,7 @@
         <v>34</v>
       </c>
       <c r="B21" s="64">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="C21" s="65"/>
       <c r="D21" s="64">
@@ -1392,7 +1392,7 @@
         <v>36</v>
       </c>
       <c r="B23" s="64">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C23" s="65"/>
       <c r="D23" s="64">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="B24" s="66">
         <f>B21*(B22-B23)</f>
-        <v>400000</v>
+        <v>500000</v>
       </c>
       <c r="C24" s="67"/>
       <c r="D24" s="66">

</xml_diff>